<commit_message>
update class diagram and functions
</commit_message>
<xml_diff>
--- a/3-Design/High Level Design/class diagram.xlsx
+++ b/3-Design/High Level Design/class diagram.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73EA065-2CF8-48AB-9318-A4ED10C3DC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t xml:space="preserve">       +     Resgister( )</t>
   </si>
@@ -93,21 +103,6 @@
     <t>Restaurant menu page</t>
   </si>
   <si>
-    <t xml:space="preserve">       +     View restaurant name ( )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       +     View item description ( )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       +     View price items ( )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       +     Increase quantity item ( )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       +     Decrease quantity item ( )</t>
-  </si>
-  <si>
     <t xml:space="preserve">       +     Place order ( )</t>
   </si>
   <si>
@@ -135,15 +130,6 @@
     <t>-        Loyalty points : int</t>
   </si>
   <si>
-    <t xml:space="preserve">       +     View order name ( )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       +     View order quantity ( )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       +     View total price ( )</t>
-  </si>
-  <si>
     <t xml:space="preserve">       +     View delivery address ( )</t>
   </si>
   <si>
@@ -214,12 +200,21 @@
   </si>
   <si>
     <t xml:space="preserve"> -         ID : int</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       +     View restaurant data ( )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       +     View item data ( )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,10 +355,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -378,22 +372,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -414,6 +404,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +441,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="44" name="Elbow Connector 43"/>
+        <xdr:cNvPr id="44" name="Elbow Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -485,9 +484,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1245219</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>18585</xdr:rowOff>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>231321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
@@ -497,13 +496,19 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Straight Arrow Connector 50"/>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13297829" y="2574073"/>
-          <a:ext cx="0" cy="390293"/>
+          <a:off x="17430750" y="2585357"/>
+          <a:ext cx="6969" cy="1456628"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -544,7 +549,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="Straight Arrow Connector 51"/>
+        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -591,7 +602,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="64" name="Straight Connector 63"/>
+        <xdr:cNvPr id="64" name="Straight Connector 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -636,7 +653,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="Straight Connector 65"/>
+        <xdr:cNvPr id="66" name="Straight Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -681,7 +704,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="Straight Arrow Connector 67"/>
+        <xdr:cNvPr id="68" name="Straight Arrow Connector 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -728,7 +757,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="71" name="Straight Arrow Connector 70"/>
+        <xdr:cNvPr id="71" name="Straight Arrow Connector 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -775,7 +810,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Straight Arrow Connector 74"/>
+        <xdr:cNvPr id="75" name="Straight Arrow Connector 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -822,7 +863,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="81" name="Straight Connector 80"/>
+        <xdr:cNvPr id="81" name="Straight Connector 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -867,7 +914,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="96" name="Straight Connector 95"/>
+        <xdr:cNvPr id="96" name="Straight Connector 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -912,7 +965,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="98" name="Straight Arrow Connector 97"/>
+        <xdr:cNvPr id="98" name="Straight Arrow Connector 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -959,7 +1018,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1004,7 +1069,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Straight Connector 20"/>
+        <xdr:cNvPr id="21" name="Straight Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1049,7 +1120,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Straight Connector 15"/>
+        <xdr:cNvPr id="16" name="Straight Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1094,7 +1171,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Straight Connector 38"/>
+        <xdr:cNvPr id="39" name="Straight Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1139,7 +1222,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Straight Connector 33"/>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1184,7 +1273,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="Straight Connector 54"/>
+        <xdr:cNvPr id="55" name="Straight Connector 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1229,7 +1324,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="Straight Connector 58"/>
+        <xdr:cNvPr id="59" name="Straight Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1274,7 +1375,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="65" name="Straight Arrow Connector 64"/>
+        <xdr:cNvPr id="65" name="Straight Arrow Connector 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1321,7 +1428,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="69" name="Straight Arrow Connector 68"/>
+        <xdr:cNvPr id="69" name="Straight Arrow Connector 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1368,7 +1481,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Straight Arrow Connector 78"/>
+        <xdr:cNvPr id="79" name="Straight Arrow Connector 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1665,404 +1784,377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E2:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="35.77734375" customWidth="1"/>
-    <col min="8" max="8" width="38.5546875" customWidth="1"/>
-    <col min="9" max="9" width="32.77734375" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="5:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="19" t="s">
+    <row r="2" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="5:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="1"/>
+      <c r="K3" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="5:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="15"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="17"/>
+      <c r="K5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="5:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="15"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="9"/>
+      <c r="K12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="18" spans="5:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="17"/>
+      <c r="I21" s="19"/>
+      <c r="K21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="5:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="15"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="15"/>
+      <c r="F28" s="13"/>
+      <c r="I28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="I29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="I30" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+    </row>
+    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+    </row>
+    <row r="33" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+    </row>
+    <row r="34" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+    </row>
+    <row r="35" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="2"/>
-      <c r="K3" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="5:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="20"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="5:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="22"/>
-      <c r="K5" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="5:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="5:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="5:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="1"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="5:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="20"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="10"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="5:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="10"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="5:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="5:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="5:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F17" s="15"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F18" s="15"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="15"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="15"/>
-      <c r="G20" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="5:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="20"/>
-      <c r="M21" s="20"/>
-    </row>
-    <row r="22" spans="5:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="20"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="5:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="5:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="5:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="14"/>
-      <c r="G25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="5:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="15"/>
-      <c r="G26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="5:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="5:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="20"/>
-      <c r="F28" s="18"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="5:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="5:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="K30" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="5:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="11"/>
-      <c r="K31" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="5:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="K32" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="11:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="K33" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K34" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E60" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>